<commit_message>
fixed HashTable for csv
</commit_message>
<xml_diff>
--- a/WGUPS Distance Table.xlsx
+++ b/WGUPS Distance Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\C950 DSA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CAEC592-F421-441E-8A78-91BE272EE8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015F9676-6C00-47D7-84AB-E9DA6FBA5E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -226,10 +226,6 @@
  5383 South 900 East #104</t>
   </si>
   <si>
-    <t xml:space="preserve"> 5383 S 900 East #104
-(84117)</t>
-  </si>
-  <si>
     <t>Rice Terrace Pavilion Park
  600 E 900 South</t>
   </si>
@@ -250,6 +246,10 @@
   </si>
   <si>
     <t>NHP2: WGUPS Routing Program</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5383 South 900 East #104
+(84117)</t>
   </si>
 </sst>
 </file>
@@ -961,19 +961,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.08984375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="29" width="5.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="29" width="5.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
       <c r="E1" s="23"/>
@@ -985,7 +985,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
@@ -997,7 +997,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
@@ -1009,7 +1009,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="24" t="s">
         <v>0</v>
       </c>
@@ -1035,7 +1035,7 @@
       <c r="V4" s="25"/>
       <c r="W4" s="25"/>
     </row>
-    <row r="5" spans="1:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
@@ -1059,9 +1059,9 @@
       <c r="V5" s="25"/>
       <c r="W5" s="25"/>
     </row>
-    <row r="6" spans="1:29" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:29" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="26"/>
       <c r="E6" s="26"/>
@@ -1078,7 +1078,7 @@
       <c r="P6" s="25"/>
       <c r="Q6" s="25"/>
     </row>
-    <row r="7" spans="1:29" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:29" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -1086,9 +1086,9 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:29" ht="160.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:29" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="22" t="s">
@@ -1167,13 +1167,13 @@
         <v>49</v>
       </c>
       <c r="AB8" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AC8" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="48" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:29" ht="48" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>1</v>
       </c>
@@ -1210,7 +1210,7 @@
       <c r="AB9" s="8"/>
       <c r="AC9" s="9"/>
     </row>
-    <row r="10" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:29" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>3</v>
       </c>
@@ -1249,7 +1249,7 @@
       <c r="AB10" s="4"/>
       <c r="AC10" s="10"/>
     </row>
-    <row r="11" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:29" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>5</v>
       </c>
@@ -1290,7 +1290,7 @@
       <c r="AB11" s="4"/>
       <c r="AC11" s="10"/>
     </row>
-    <row r="12" spans="1:29" ht="36" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:29" ht="36" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>7</v>
       </c>
@@ -1333,7 +1333,7 @@
       <c r="AB12" s="4"/>
       <c r="AC12" s="10"/>
     </row>
-    <row r="13" spans="1:29" ht="36" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:29" ht="36" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>9</v>
       </c>
@@ -1378,7 +1378,7 @@
       <c r="AB13" s="4"/>
       <c r="AC13" s="10"/>
     </row>
-    <row r="14" spans="1:29" ht="36" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:29" ht="36" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>11</v>
       </c>
@@ -1425,7 +1425,7 @@
       <c r="AB14" s="4"/>
       <c r="AC14" s="10"/>
     </row>
-    <row r="15" spans="1:29" ht="36" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:29" ht="36" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>13</v>
       </c>
@@ -1474,7 +1474,7 @@
       <c r="AB15" s="4"/>
       <c r="AC15" s="10"/>
     </row>
-    <row r="16" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:29" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>15</v>
       </c>
@@ -1525,7 +1525,7 @@
       <c r="AB16" s="4"/>
       <c r="AC16" s="10"/>
     </row>
-    <row r="17" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:29" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>17</v>
       </c>
@@ -1578,7 +1578,7 @@
       <c r="AB17" s="4"/>
       <c r="AC17" s="10"/>
     </row>
-    <row r="18" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:29" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>19</v>
       </c>
@@ -1633,7 +1633,7 @@
       <c r="AB18" s="4"/>
       <c r="AC18" s="10"/>
     </row>
-    <row r="19" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:29" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>21</v>
       </c>
@@ -1690,7 +1690,7 @@
       <c r="AB19" s="4"/>
       <c r="AC19" s="10"/>
     </row>
-    <row r="20" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:29" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>23</v>
       </c>
@@ -1749,7 +1749,7 @@
       <c r="AB20" s="4"/>
       <c r="AC20" s="10"/>
     </row>
-    <row r="21" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:29" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>25</v>
       </c>
@@ -1810,7 +1810,7 @@
       <c r="AB21" s="4"/>
       <c r="AC21" s="10"/>
     </row>
-    <row r="22" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:29" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>27</v>
       </c>
@@ -1873,7 +1873,7 @@
       <c r="AB22" s="4"/>
       <c r="AC22" s="10"/>
     </row>
-    <row r="23" spans="1:29" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:29" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>29</v>
       </c>
@@ -1938,7 +1938,7 @@
       <c r="AB23" s="4"/>
       <c r="AC23" s="10"/>
     </row>
-    <row r="24" spans="1:29" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:29" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>31</v>
       </c>
@@ -2005,7 +2005,7 @@
       <c r="AB24" s="4"/>
       <c r="AC24" s="10"/>
     </row>
-    <row r="25" spans="1:29" ht="36" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:29" ht="48" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>33</v>
       </c>
@@ -2074,7 +2074,7 @@
       <c r="AB25" s="4"/>
       <c r="AC25" s="10"/>
     </row>
-    <row r="26" spans="1:29" ht="36" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:29" ht="36" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>35</v>
       </c>
@@ -2145,7 +2145,7 @@
       <c r="AB26" s="4"/>
       <c r="AC26" s="10"/>
     </row>
-    <row r="27" spans="1:29" ht="36" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:29" ht="36" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>37</v>
       </c>
@@ -2218,7 +2218,7 @@
       <c r="AB27" s="4"/>
       <c r="AC27" s="10"/>
     </row>
-    <row r="28" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:29" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>39</v>
       </c>
@@ -2293,7 +2293,7 @@
       <c r="AB28" s="4"/>
       <c r="AC28" s="10"/>
     </row>
-    <row r="29" spans="1:29" ht="36" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:29" ht="36" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>41</v>
       </c>
@@ -2370,7 +2370,7 @@
       <c r="AB29" s="4"/>
       <c r="AC29" s="10"/>
     </row>
-    <row r="30" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:29" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>43</v>
       </c>
@@ -2449,7 +2449,7 @@
       <c r="AB30" s="4"/>
       <c r="AC30" s="10"/>
     </row>
-    <row r="31" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:29" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>45</v>
       </c>
@@ -2530,7 +2530,7 @@
       <c r="AB31" s="4"/>
       <c r="AC31" s="10"/>
     </row>
-    <row r="32" spans="1:29" ht="36" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:29" ht="36" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>47</v>
       </c>
@@ -2613,12 +2613,12 @@
       <c r="AB32" s="4"/>
       <c r="AC32" s="10"/>
     </row>
-    <row r="33" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:29" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C33" s="5">
         <v>2.4</v>
@@ -2698,12 +2698,12 @@
       <c r="AB33" s="4"/>
       <c r="AC33" s="10"/>
     </row>
-    <row r="34" spans="1:29" ht="24" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:29" ht="36" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="19" t="s">
         <v>51</v>
-      </c>
-      <c r="B34" s="19" t="s">
-        <v>52</v>
       </c>
       <c r="C34" s="5">
         <v>5</v>
@@ -2785,12 +2785,12 @@
       </c>
       <c r="AC34" s="10"/>
     </row>
-    <row r="35" spans="1:29" ht="23.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:29" ht="23.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="20" t="s">
         <v>53</v>
-      </c>
-      <c r="B35" s="20" t="s">
-        <v>54</v>
       </c>
       <c r="C35" s="11">
         <v>3.6</v>
@@ -2887,64 +2887,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Launch_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Discipline xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Course_x0020_code xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Performance_x0020_Steps_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <Value>N/A</Value>
-    </Performance_x0020_Steps_x0020_Completed>
-    <Course_x0020_short_x0020_name xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Course_x0020_number xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Course_x0020_title xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <d5fh xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Step_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <Value>N/A</Value>
-    </Step_x0020_Completed>
-    <Publication_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <SME xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Editor0 xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Editor0>
-    <Doc_x0020_Type xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <qrac xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Specifications xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Clone xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <AssessmentType xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <AssessmentCode xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <PDO xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </PDO>
-    <TaxCatchAll xmlns="1f707338-ea0f-4fe5-baee-59b996692b22" xsi:nil="true"/>
-    <_x0033_rdPartyCertVendor xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C39F2A75005F2D43B30369DAED2CCB1C" ma:contentTypeVersion="51" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dca2bb0f68bdf94cc5f80c9292ca56b2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xmlns:ns3="1f707338-ea0f-4fe5-baee-59b996692b22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d4cb8629785915e947a4406c57312ba8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3454,7 +3396,93 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Launch_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Discipline xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Course_x0020_code xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Performance_x0020_Steps_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <Value>N/A</Value>
+    </Performance_x0020_Steps_x0020_Completed>
+    <Course_x0020_short_x0020_name xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Course_x0020_number xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Course_x0020_title xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <d5fh xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Step_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <Value>N/A</Value>
+    </Step_x0020_Completed>
+    <Publication_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <SME xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Editor0 xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Editor0>
+    <Doc_x0020_Type xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <qrac xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Specifications xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Clone xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <AssessmentType xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <AssessmentCode xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <PDO xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </PDO>
+    <TaxCatchAll xmlns="1f707338-ea0f-4fe5-baee-59b996692b22" xsi:nil="true"/>
+    <_x0033_rdPartyCertVendor xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{346B5534-CC83-47DD-8523-BB97FB1B43B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
+    <ds:schemaRef ds:uri="1f707338-ea0f-4fe5-baee-59b996692b22"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51ED99C8-D91C-4521-83EC-2A0A02D58674}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC12B168-B9E1-4151-98F9-C97DA1AB8BBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="e7b1d905-24de-49f1-ac69-282527225b8e"/>
@@ -3472,32 +3500,4 @@
     <ds:schemaRef ds:uri="1f707338-ea0f-4fe5-baee-59b996692b22"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51ED99C8-D91C-4521-83EC-2A0A02D58674}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{346B5534-CC83-47DD-8523-BB97FB1B43B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
-    <ds:schemaRef ds:uri="1f707338-ea0f-4fe5-baee-59b996692b22"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>